<commit_message>
Added question for eligibility checker
</commit_message>
<xml_diff>
--- a/Data Files/Portal_Verification.xlsx
+++ b/Data Files/Portal_Verification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Data-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE6460D-17F8-4765-BF8E-B136323ED325}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5C26DE-017D-47F0-AFAA-906FF1639B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>Does your appeal relate to a listed building?</t>
   </si>
@@ -468,6 +468,9 @@
   <si>
     <t>If you know the names and addresses of some, but not all, of the owners of the land involved in the appeal, you must serve notice on the owners that you do know about. You must also publish the notice in a local newspaper. This is so that any other owners may become aware of your intention to appeal.
 In these circumstances you should complete this certificate . This is an editable document which needs to be saved and uploaded to the appeal form and upload a copy of it, and the notice as published, with your appeal form.</t>
+  </si>
+  <si>
+    <t>What was the outcome of your application?</t>
   </si>
 </sst>
 </file>
@@ -825,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192F818B-9F99-4506-AB8C-E6CF706CA6D3}">
-  <dimension ref="A1:A90"/>
+  <dimension ref="A1:A91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1286,6 +1289,11 @@
         <v>88</v>
       </c>
     </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New Portal Verification data
</commit_message>
<xml_diff>
--- a/Data Files/Portal_Verification.xlsx
+++ b/Data Files/Portal_Verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Data-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5C26DE-017D-47F0-AFAA-906FF1639B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FD2A26-75C7-4DE5-8CEE-63EE10144BEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
   </bookViews>
@@ -36,12 +36,6 @@
     <t>Does your appeal relate to a listed building?</t>
   </si>
   <si>
-    <t>Have you received a decision from the Local Planning Authority?</t>
-  </si>
-  <si>
-    <t>Did you make the original application under the Householder Application Service? This will include, for example, an extension to a single existing house.</t>
-  </si>
-  <si>
     <t>What type of planning permission did you apply for?</t>
   </si>
   <si>
@@ -60,9 +54,6 @@
     <t>Is there a dispute over local list documentation?</t>
   </si>
   <si>
-    <t>Eligibility confirmed</t>
-  </si>
-  <si>
     <t>Did you submit your application more than 8 weeks ago?</t>
   </si>
   <si>
@@ -72,43 +63,10 @@
     <t>No right to appeal</t>
   </si>
   <si>
-    <t>What does your appeal relate to?</t>
-  </si>
-  <si>
     <t>Please enter your username and password to continue.</t>
   </si>
   <si>
     <t xml:space="preserve">Welcome to the Planning Inspectorate site </t>
-  </si>
-  <si>
-    <t>Is the site address within one of the following Local Planning Authorities:
-Adur District Council
-Arun District Council
-Ashford Borough Council
-Brighton and Hove City Council
-Canterbury City Council
-Chichester District Council
-Crawley Borough Council
-Dartford Borough Council
-Dover District Council
-East Sussex County Council
-Eastbourne Borough Council
-Folkestone and Hythe District Council
-Gravesham Borough Council
-Hastings Borough Council
-Horsham District Council
-Kent County Council
-Lewes District Council
-Maidstone Borough Council
-Medway Council
-Mid Sussex District Council
-Rother District Council
-Sevenoaks District Council
-South Downs National Park authority
-Swale Borough Council
-Tunbridge Wells Borough Council
-West Sussex County Council
-Worthing Borough Council</t>
   </si>
   <si>
     <t>Do you have an account?</t>
@@ -420,9 +378,6 @@
 Get application as PDF</t>
   </si>
   <si>
-    <t>Are you happy for your appeal to be decided using the written representation or hearing procedure?</t>
-  </si>
-  <si>
     <t>APPEAL SUBMITTED</t>
   </si>
   <si>
@@ -468,6 +423,52 @@
   <si>
     <t>If you know the names and addresses of some, but not all, of the owners of the land involved in the appeal, you must serve notice on the owners that you do know about. You must also publish the notice in a local newspaper. This is so that any other owners may become aware of your intention to appeal.
 In these circumstances you should complete this certificate . This is an editable document which needs to be saved and uploaded to the appeal form and upload a copy of it, and the notice as published, with your appeal form.</t>
+  </si>
+  <si>
+    <t>Are you happy for your appeal to be decided using either written representations or a hearing?</t>
+  </si>
+  <si>
+    <t>Is the site address in one of these Local Planning Authorities?
+Adur District Council
+Arun District Council
+Ashford Borough Council
+Brighton and Hove City Council
+Canterbury City Council
+Chichester District Council
+Crawley Borough Council
+Dartford Borough Council
+Dover District Council
+East Sussex County Council
+Eastbourne Borough Council
+Folkestone and Hythe District Council
+Gravesham Borough Council
+Hastings Borough Council
+Horsham District Council
+Kent County Council
+Lewes District Council
+Maidstone Borough Council
+Medway Council
+Mid Sussex District Council
+Rother District Council
+Sevenoaks District Council
+South Downs National Park authority
+Swale Borough Council
+Tunbridge Wells Borough Council
+West Sussex County Council
+Worthing Borough Council</t>
+  </si>
+  <si>
+    <t>Have you received a decision notice from the Local Planning Authority?</t>
+  </si>
+  <si>
+    <t>What’s your appeal about?</t>
+  </si>
+  <si>
+    <t>Did you make the original application through the Householder Application Service?
+This would include, for example, an extension to a single existing house.</t>
+  </si>
+  <si>
+    <t>You are eligible to appeal</t>
   </si>
   <si>
     <t>What was the outcome of your application?</t>
@@ -830,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192F818B-9F99-4506-AB8C-E6CF706CA6D3}">
   <dimension ref="A1:A91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
       <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
@@ -841,12 +842,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -856,437 +857,437 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>2</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="360" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="144" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Started 845 appeals scenario 1
</commit_message>
<xml_diff>
--- a/Data Files/Portal_Verification.xlsx
+++ b/Data Files/Portal_Verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Data-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FD2A26-75C7-4DE5-8CEE-63EE10144BEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E83EF2E-40B4-478E-9B95-6824F954AC0F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Verifications" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
   <si>
     <t>Does your appeal relate to a listed building?</t>
   </si>
@@ -39,30 +39,12 @@
     <t>What type of planning permission did you apply for?</t>
   </si>
   <si>
-    <t>Have you been served with an enforcement notice?</t>
-  </si>
-  <si>
     <t>What's the date on the decision notice?</t>
   </si>
   <si>
-    <t>You have passed the deadline date for appealing</t>
-  </si>
-  <si>
-    <t>You're not eligible to use the beta service</t>
-  </si>
-  <si>
-    <t>Is there a dispute over local list documentation?</t>
-  </si>
-  <si>
     <t>Did you submit your application more than 8 weeks ago?</t>
   </si>
   <si>
-    <t>Was there an agreement with the LPA to extend the application decision period?</t>
-  </si>
-  <si>
-    <t>No right to appeal</t>
-  </si>
-  <si>
     <t>Please enter your username and password to continue.</t>
   </si>
   <si>
@@ -100,14 +82,6 @@
   </si>
   <si>
     <t>Upload the planning application form</t>
-  </si>
-  <si>
-    <t>Planning application form
-LPA decision notice (unless this refers to a non-determination appeal)
-Application reference (from the LPA decision notice)
-Plans upon which the LPA made their decision (if applicable)
-Any other relevant plans (if applicable)
-Grounds for appeal</t>
   </si>
   <si>
     <t>Upload the LPA decision notice</t>
@@ -219,9 +193,6 @@
   </si>
   <si>
     <t>Upload any documents to support your statement</t>
-  </si>
-  <si>
-    <t>Is there another ongoing appeal that relates to this site?</t>
   </si>
   <si>
     <t>Do you intend to submit another planning appeal that relates to this site?</t>
@@ -381,15 +352,6 @@
     <t>APPEAL SUBMITTED</t>
   </si>
   <si>
-    <t>When did you receive your decision?</t>
-  </si>
-  <si>
-    <t>On what date was the planning obligation made?</t>
-  </si>
-  <si>
-    <t>What is the date on the decision notice?</t>
-  </si>
-  <si>
     <t>What conditions are you appealing against?</t>
   </si>
   <si>
@@ -428,7 +390,46 @@
     <t>Are you happy for your appeal to be decided using either written representations or a hearing?</t>
   </si>
   <si>
+    <t>Have you received a decision notice from the Local Planning Authority?</t>
+  </si>
+  <si>
+    <t>What’s your appeal about?</t>
+  </si>
+  <si>
+    <t>Did you make the original application through the Householder Application Service?
+This would include, for example, an extension to a single existing house.</t>
+  </si>
+  <si>
+    <t>You are eligible to appeal</t>
+  </si>
+  <si>
+    <t>What was the outcome of your application?</t>
+  </si>
+  <si>
+    <t>You need to use our existing service</t>
+  </si>
+  <si>
+    <t>Have you been served with an enforcement notice?</t>
+  </si>
+  <si>
+    <t>The deadline for appeal has passed</t>
+  </si>
+  <si>
+    <t>Is there a dispute over local list documentation?
+Each Local Planning Authority (LPA) has a ‘local list’ of documents needed for an application.</t>
+  </si>
+  <si>
+    <t>Was there an agreement with the Local Planning Authority to extend the decision date?</t>
+  </si>
+  <si>
+    <t>You cannot appeal</t>
+  </si>
+  <si>
+    <t>What date was the planning obligation made on?</t>
+  </si>
+  <si>
     <t>Is the site address in one of these Local Planning Authorities?
+Site address refers to the building or site listed in the original planning application.
 Adur District Council
 Arun District Council
 Ashford Borough Council
@@ -458,20 +459,15 @@
 Worthing Borough Council</t>
   </si>
   <si>
-    <t>Have you received a decision notice from the Local Planning Authority?</t>
-  </si>
-  <si>
-    <t>What’s your appeal about?</t>
-  </si>
-  <si>
-    <t>Did you make the original application through the Householder Application Service?
-This would include, for example, an extension to a single existing house.</t>
-  </si>
-  <si>
-    <t>You are eligible to appeal</t>
-  </si>
-  <si>
-    <t>What was the outcome of your application?</t>
+    <t>Your grounds for appeal
+Planning application form
+Decision notice from your Local Planning Authority (LPA) (unless it is a non-determination appeal)
+Application reference (from the LPA decision notice)
+The plans on which the LPA made their decision (optional)
+Any other relevant plans (optional)</t>
+  </si>
+  <si>
+    <t>Do you have other ongoing appeals related to this site?</t>
   </si>
 </sst>
 </file>
@@ -831,468 +827,468 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192F818B-9F99-4506-AB8C-E6CF706CA6D3}">
   <dimension ref="A1:A91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="207.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="207.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="14" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="20" spans="1:1" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="403.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="145" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="360" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" ht="144" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="89" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
+    <row r="90" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed 847 scenario 1
</commit_message>
<xml_diff>
--- a/Data Files/Portal_Verification.xlsx
+++ b/Data Files/Portal_Verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Data-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39CB484-7BDA-4529-8EE8-3A92CB6D3EC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F625DBA-CF9A-49E8-B8B8-46634909EF9D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Verifications" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
   <si>
     <t>Does your appeal relate to a listed building?</t>
   </si>
@@ -485,6 +485,12 @@
   </si>
   <si>
     <t>Upload any documents relevant to the dispute of local list documentation</t>
+  </si>
+  <si>
+    <t>Upload a copy of the LPA planning decision showing approval of the outline planning permission</t>
+  </si>
+  <si>
+    <t>Upload a copy of the LPA decision notice that you are appealing against</t>
   </si>
 </sst>
 </file>
@@ -849,490 +855,500 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192F818B-9F99-4506-AB8C-E6CF706CA6D3}">
-  <dimension ref="A1:A95"/>
+  <dimension ref="A1:A97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="207.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="207.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="360" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="375" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" ht="315" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" ht="285" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="144" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" ht="150" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added excel file into data files
</commit_message>
<xml_diff>
--- a/Data Files/Portal_Verification.xlsx
+++ b/Data Files/Portal_Verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Data-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584AB33A-17AC-49AA-8826-2090FE787B55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1B9662-6A9A-4B90-A707-816A3334B9D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Verifications" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="116">
   <si>
     <t>Does your appeal relate to a listed building?</t>
   </si>
@@ -236,9 +236,6 @@
 sexual orientation</t>
   </si>
   <si>
-    <t>Do you wish to submit an application for costs with this appeal?</t>
-  </si>
-  <si>
     <t>You can claim costs if someone involved in your planning appeal behaves unreasonably and costs you money.
 You make a claim for an ‘award of costs’ to the Planning Inspectorate. If you’re successful, you’ll have to reach an agreement with the other party about how much they pay.
 You can be asked to pay costs if you behave unreasonably during your own appeal. The Planning Inspectorate can do this even if nobody’s claiming costs against you.</t>
@@ -297,9 +294,6 @@
   </si>
   <si>
     <t>By submitting this appeal you are confirming that, to the best of your knowledge, the details you are providing are correct.</t>
-  </si>
-  <si>
-    <t>We'll validate your appeal and pass it to an Inspector. You'll be allocated a names case officer who will write to you to start the appeal and set out details of the timetable and procedure.</t>
   </si>
   <si>
     <t>You can sign in to your Planning Inspectorate account at any time to track your appeal.</t>
@@ -520,10 +514,79 @@
     <t>Upload the planning application form or application letter</t>
   </si>
   <si>
-    <t>Provide a brief summary of why you think the inquiry procedure is appropriate</t>
-  </si>
-  <si>
-    <t>Upload a draft statement of common ground</t>
+    <t>Provide a copy of the original planning decision showing the condition applied by the LPA</t>
+  </si>
+  <si>
+    <t>Why the planning application was refused
+Select all reasons that the LPA gave when refusing permission to vary or remove the condition
+Affordable housing
+Agricultural need
+Character and appearance of a National Park or AONB
+Character and appearance of a conservation area
+Other character and appearance and visual impact
+Drainage
+Flooding
+Highway safety
+Human rights
+Impact on a protected species
+Impact on a SSSI, SPA, Ramsar or habitat
+Inappropriate development in a green belt
+Landscaping
+Listed building or scheduled ancient monuments
+Living conditions
+Noise
+Pollution
+Power generation/energy saving
+Retail vitality and viability
+Shadow flicker
+Tree Preservation Order
+Other
+If the reason for refusal given in your planning decision letter is not listed, select Other and state the reasons given.</t>
+  </si>
+  <si>
+    <t>Have you published your intention to appeal in a local newspaper, where all land owners of the holding are likely to have seen it?</t>
+  </si>
+  <si>
+    <t>We'll validate your appeal and pass it to an Inspector. You'll be allocated a named case officer who will write to you to start the appeal and set out details of the timetable and procedure.</t>
+  </si>
+  <si>
+    <t>Why the planning application was refused
+Select all reasons that the LPA gave when refusing prior approval of permitted development rights
+Not suitable for permitted development rights
+Does not fall under permitted development rights
+Exceeded the permitted development rights
+Other
+If the reason for refusal given in your planning decision letter is not listed, select Other and state the reasons given.</t>
+  </si>
+  <si>
+    <t>Provide any evidence the LPA have notified the neighbours to the affected land (either side and behind the property)</t>
+  </si>
+  <si>
+    <t>Do you wish to submit an application for costs with this appeal?</t>
+  </si>
+  <si>
+    <t>Do you wish to submit an application for costs with this appeal form?</t>
+  </si>
+  <si>
+    <t>Did you submit your application more than 5 weeks ago?</t>
+  </si>
+  <si>
+    <t>Will the change of use be creating any additional residential dwellings?</t>
+  </si>
+  <si>
+    <t>Do you know the proposed number of residential dwellings?</t>
+  </si>
+  <si>
+    <t>Provide the revised description of the development</t>
+  </si>
+  <si>
+    <t>Why has the description of the development changed?</t>
+  </si>
+  <si>
+    <t>For HAS/CAS appeals, if you are intending to submit a costs application, please do so now as there is no provision later in the appeal process</t>
+  </si>
+  <si>
+    <t>Are the landowners aware, and have they consented to, the placement of the advertisement?</t>
   </si>
 </sst>
 </file>
@@ -888,555 +951,610 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192F818B-9F99-4506-AB8C-E6CF706CA6D3}">
-  <dimension ref="A1:A108"/>
+  <dimension ref="A1:A119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="207.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="207.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="87" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="87" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="360" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" ht="116" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:1" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="145" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" ht="144" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    <row r="75" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+    <row r="85" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="3" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+    <row r="108" spans="1:1" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A108" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>104</v>
+    <row r="110" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Script changes and new test suite for pre-prod run.
</commit_message>
<xml_diff>
--- a/Data Files/Portal_Verification.xlsx
+++ b/Data Files/Portal_Verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Data-Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AutoTest_1\git\PINS_ODT_TEST\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584AB33A-17AC-49AA-8826-2090FE787B55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5522C164-3F7E-4DEE-9338-21B0AE078B05}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Verifications" sheetId="1" r:id="rId1"/>
@@ -130,29 +130,6 @@
   </si>
   <si>
     <t>Upload any technical reports that you submitted as part of the planning application</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                        Select technical report type
-                        Arboricultural report
-                        Transport or Traffic Impact Assessment
-                        Noise Assessment
-                        Archaeological report
-                        Retail Assessment
-                        Flood Risk Assessment
-                        Environmental Statement
-                        Agricultural Appraisal
-                        Radio Emissions -telecomms
-                        Air Quality Assessment
-                        Urban Capacity Studies
-                        Habitat
-                        Protected Species
-                        Contamination/stability
-                        Landscape assessment (C&amp;A)
-                        Daylight Report (LC)
-                        Viability Report/ Business Plans
-                        Shadow Flicker Report
-                        Section 106 Agreement
-                        Other reports</t>
   </si>
   <si>
     <t>Does the site have a postcode</t>
@@ -524,6 +501,29 @@
   </si>
   <si>
     <t>Upload a draft statement of common ground</t>
+  </si>
+  <si>
+    <t>Select technical report type
+Arboricultural report
+Transport or Traffic Impact Assessment
+Noise Assessment
+Archaeological report
+Retail Assessment
+Flood Risk Assessment
+Environmental Statement
+Agricultural Appraisal
+Radio Emissions -telecomms
+Air Quality Assessment
+Urban Capacity Studies
+Habitat
+Protected Species
+Contamination/stability
+Landscape assessment (C&amp;A)
+Daylight Report (LC)
+Viability Report/ Business Plans
+Shadow Flicker Report
+Section 106 Agreement
+Other reports</t>
   </si>
 </sst>
 </file>
@@ -565,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -574,6 +574,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -890,553 +893,553 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192F818B-9F99-4506-AB8C-E6CF706CA6D3}">
   <dimension ref="A1:A108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="207.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="207.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="87" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="87" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="360" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:1" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="51" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="55" spans="1:1" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="57" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:1" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="145" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" ht="144" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="85" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="3" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Tests added for Appeal type 852.
</commit_message>
<xml_diff>
--- a/Data Files/Portal_Verification.xlsx
+++ b/Data Files/Portal_Verification.xlsx
@@ -1,6 +1,37 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AutoTest_1\git\PINS_ODT_TEST\Data Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB65E32-A095-4263-B717-02F200BA9B91}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Verifications" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
+</workbook>
+</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="117">
   <si>
     <t>Does your appeal relate to a listed building?</t>
   </si>
@@ -556,6 +587,34 @@
   </si>
   <si>
     <t>Are the landowners aware, and have they consented to, the placement of the advertisement?</t>
+  </si>
+  <si>
+    <t>Why the planning application was refused
+Select all reasons that the LPA gave when refusing planning permission
+Affordable housing
+Agricultural need
+Character and appearance of a National Park or AONB
+Character and appearance of a conservation area
+Other character and appearance and visual impact
+Drainage
+Flooding
+Highway safety
+Human rights
+Impact on a protected species
+Impact on a SSSI, SPA, Ramsar or habitat
+Inappropriate development in a green belt
+Landscaping
+Listed building or scheduled ancient monuments
+Living conditions
+Noise
+Pollution
+Power generation/energy saving
+Retail vitality and viability
+Shadow flicker
+Tree Preservation Order
+Other
+None applicable
+If the reason for refusal given in your planning decision letter is not listed, select Other and state the reasons given.</t>
   </si>
 </sst>
 </file>
@@ -621,4 +680,918 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192F818B-9F99-4506-AB8C-E6CF706CA6D3}">
+  <dimension ref="A1:A120"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="207.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="145" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="116" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A108" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" ht="377" x14ac:dyDescent="0.35">
+      <c r="A120" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed question 4 hidden questions test
</commit_message>
<xml_diff>
--- a/Data Files/Portal_Verification.xlsx
+++ b/Data Files/Portal_Verification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon\Data-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1006F4-2CE1-4B17-A319-0A09378DB628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA13019-694E-4BC9-9E6C-3679CEC1D9C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="164">
   <si>
     <t>Does your appeal relate to a listed building?</t>
   </si>
@@ -665,28 +665,109 @@
     <t>You can now submit your application on the grounds of: Other</t>
   </si>
   <si>
+    <t>You can now submit your application on the grounds of: Refused permission to vary or remove a condition(s) (Technical Design)</t>
+  </si>
+  <si>
+    <t>You can now submit your application on the grounds of: Non-determination appeal (Permission in Principle)</t>
+  </si>
+  <si>
+    <t>You can now submit your application on the grounds of: Non-determination appeal (Technical Design)</t>
+  </si>
+  <si>
+    <t>You can now submit your application on the grounds of: HAS Prior approval</t>
+  </si>
+  <si>
+    <t>You can now submit your application on the grounds of: Refused to approve any matter required by a condition on a previous planning permission</t>
+  </si>
+  <si>
+    <t>You can now submit your application on the grounds of: Permission in Principle</t>
+  </si>
+  <si>
+    <t>You can now submit your application on the grounds of: Technical Design Consent</t>
+  </si>
+  <si>
+    <t>If you submitted any plans that differ from those the LPA made their decision on, upload them here.</t>
+  </si>
+  <si>
+    <t>Upload any other plans you haven't yet submitted, but you feel are relevant to the application.</t>
+  </si>
+  <si>
+    <t>Is any part of the appeal site within the Green Belt?</t>
+  </si>
+  <si>
+    <t>Was your application for</t>
+  </si>
+  <si>
+    <t>Upload any technical reports you have produced since making the planning application</t>
+  </si>
+  <si>
+    <t>If you submitted any plans to the LPA that differ from those used in your planning application, upload them here</t>
+  </si>
+  <si>
     <t>You can now submit your application on the grounds of: Granted planning permission for the development subject to conditions to which you object (Technical Design)</t>
   </si>
   <si>
-    <t>You can now submit your application on the grounds of: Refused permission to vary or remove a condition(s) (Technical Design)</t>
-  </si>
-  <si>
-    <t>You can now submit your application on the grounds of: Non-determination appeal (Permission in Principle)</t>
-  </si>
-  <si>
-    <t>You can now submit your application on the grounds of: Non-determination appeal (Technical Design)</t>
-  </si>
-  <si>
-    <t>You can now submit your application on the grounds of: HAS Prior approval</t>
-  </si>
-  <si>
-    <t>You can now submit your application on the grounds of: Refused to approve any matter required by a condition on a previous planning permission</t>
-  </si>
-  <si>
-    <t>You can now submit your application on the grounds of: Permission in Principle</t>
-  </si>
-  <si>
-    <t>You can now submit your application on the grounds of: Technical Design Consent</t>
+    <t>How have you measured the scale of the site?</t>
+  </si>
+  <si>
+    <t>How many tonnes will be incinerated per year?</t>
+  </si>
+  <si>
+    <t>What's the scale of the proposed mineral development?</t>
+  </si>
+  <si>
+    <t>What's the scale of the proposed waste development?</t>
+  </si>
+  <si>
+    <t>Have you measured the site in hectares or square metres?</t>
+  </si>
+  <si>
+    <t>What does the proposed renewable energy development involve?</t>
+  </si>
+  <si>
+    <t>Do you intend to challenge the local planning authority’s 5 year housing land supply?</t>
+  </si>
+  <si>
+    <t>Does the proposed development relate to a House in Multiple Occupation (HMO)?</t>
+  </si>
+  <si>
+    <t>How tall is the proposed mast?</t>
+  </si>
+  <si>
+    <t>How many traveller and caravan pitches are part of the proposed development?</t>
+  </si>
+  <si>
+    <t>Yes
+No</t>
+  </si>
+  <si>
+    <t>Area (hectares)
+Floorspace (square metres)</t>
+  </si>
+  <si>
+    <t>Up to 100,000 tonnes
+Over 100,000 tonnes</t>
+  </si>
+  <si>
+    <t>Under 4 ha, 50,000 tonnes or 5 years duration
+4 to 10 ha, 50,000 to 100,000 tonnes or 5 to 10 years duration
+10 to 20 ha, 100,000 to 500,000 tonnes or 10 to 25 years duration
+Over 20 ha, over 500,000 tonnes or over 25 years duration</t>
+  </si>
+  <si>
+    <t>Turbines/anemometers
+Solar farm
+Both</t>
+  </si>
+  <si>
+    <t>Up to (and including) 20 m
+Over 20 m</t>
+  </si>
+  <si>
+    <t>1 to 3
+4 to 10
+11 to 15
+Over 15</t>
   </si>
 </sst>
 </file>
@@ -728,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -737,6 +818,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -752,6 +836,65 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D118-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>148</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>149</xdr:row>
+          <xdr:rowOff>60960</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Control 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1050,11 +1193,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192F818B-9F99-4506-AB8C-E6CF706CA6D3}">
-  <dimension ref="A1:A144"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192F818B-9F99-4506-AB8C-E6CF706CA6D3}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:A167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1704,7 +1848,7 @@
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
@@ -1749,41 +1893,185 @@
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A161" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A162" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A163" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A164" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A165" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A166" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A167" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId4" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>148</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>149</xdr:row>
+                <xdr:rowOff>60960</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New Test added for Accessibility checks.
</commit_message>
<xml_diff>
--- a/Data Files/Portal_Verification.xlsx
+++ b/Data Files/Portal_Verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AutoTest_1\git\PINS_ODT_NEW_TEST\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B39931A-7B48-4290-BA82-86C27BF5F3BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47159A01-44D7-4FD5-B70C-BEE3C10D5DE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{54CE332F-CBA2-47CB-8B23-5DC5DAF8AFDA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="171">
   <si>
     <t>Does your appeal relate to a listed building?</t>
   </si>
@@ -783,6 +783,12 @@
   </si>
   <si>
     <t>Appeal a planning decision / 848-HAS</t>
+  </si>
+  <si>
+    <t>Appeals casework portal documentation</t>
+  </si>
+  <si>
+    <t>Planning system</t>
   </si>
 </sst>
 </file>
@@ -1210,9 +1216,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192F818B-9F99-4506-AB8C-E6CF706CA6D3}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A172"/>
+  <dimension ref="A1:A174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="A173" sqref="A173"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2077,6 +2085,16 @@
     <row r="172" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A173" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>